<commit_message>
Added V. Regulator options
</commit_message>
<xml_diff>
--- a/PCB References/Hardware Overview.xlsx
+++ b/PCB References/Hardware Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-hardware/PCB References/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cam/Documents/fLoRa/flora-hardware/PCB References/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{85490C7A-8920-FC45-AB35-CE5BD8295018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F5DCF44-3EAA-4799-B05C-54D9C74FCFC5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B360BDF6-5118-D248-9D11-48712131F403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FAAE8C0D-E5AB-0842-9D3D-EA3BC991139B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{FAAE8C0D-E5AB-0842-9D3D-EA3BC991139B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
   <si>
     <t>Required Part</t>
   </si>
@@ -320,15 +320,51 @@
   <si>
     <t>Link</t>
   </si>
+  <si>
+    <t>Volatge Regulator Options</t>
+  </si>
+  <si>
+    <t>TPS78533QWDRBRQ1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/TPS78533QWDRBRQ1?qs=iLbezkQI%252BsiNbdqh2Ko9GQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/tps78533qwdrbrq1/14123967</t>
+  </si>
+  <si>
+    <t>Mouser lInk</t>
+  </si>
+  <si>
+    <t>Digi Link</t>
+  </si>
+  <si>
+    <t>LM1117MP-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/texas-instruments/LM1117MP-3-3-NOPB/304882</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Texas-Instruments/LM1117MP-3.3-NOPB?qs=X1J7HmVL2ZFn4x9DZ4T2hA%3D%3D</t>
+  </si>
+  <si>
+    <t>LDL1117S33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/stmicroelectronics/LDL1117S33R/7102071</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/STMicroelectronics/LDL1117S33R?qs=AQlKX63v8Rt9Bf6AWSrbFg%3D%3D</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -378,6 +414,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -422,7 +464,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -437,6 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +536,10 @@
     <tableColumn id="3" xr3:uid="{1AB0C512-AD43-A248-99EF-7F6AAA8DD53F}" name="Proposed Component" dataDxfId="6"/>
     <tableColumn id="15" xr3:uid="{6CD0E10F-F0BB-F04F-8AEE-C857709CD28E}" name="Vendors" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{39DF0144-5FC6-374B-AE96-8AFBF164D8C6}" name="Unit cost" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{A6916FFA-A760-4821-8413-EAD8607822E2}" name="Link" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{6D4B3BEE-02FF-8A4C-B169-44A6CECB0E18}" name="Lifecycle status" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{923E1ADB-9518-3D40-B106-467A9B15DBAE}" name="Footprint" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{0E716DA4-42E5-AB4F-B606-C4F424941A6A}" name="Justification" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A6916FFA-A760-4821-8413-EAD8607822E2}" name="Link" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{6D4B3BEE-02FF-8A4C-B169-44A6CECB0E18}" name="Lifecycle status" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{923E1ADB-9518-3D40-B106-467A9B15DBAE}" name="Footprint" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0E716DA4-42E5-AB4F-B606-C4F424941A6A}" name="Justification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -819,13 +862,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FAF2EB-E1BD-ED46-BCB0-EFDA7469991B}">
-  <dimension ref="C2:J27"/>
+  <dimension ref="C2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="0.33203125" customWidth="1"/>
@@ -833,19 +876,19 @@
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="64.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="68.25" customWidth="1"/>
+    <col min="7" max="7" width="68.1640625" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" customWidth="1"/>
     <col min="9" max="9" width="69" customWidth="1"/>
     <col min="10" max="10" width="38.33203125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="111.5">
+    <row r="2" spans="3:10" ht="100" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:10" ht="17" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -871,7 +914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="22" customHeight="1">
+    <row r="5" spans="3:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
@@ -883,7 +926,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="3:10" ht="79" customHeight="1">
+    <row r="6" spans="3:10" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
@@ -907,7 +950,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="96">
+    <row r="7" spans="3:10" ht="102" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
@@ -931,7 +974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="80">
+    <row r="8" spans="3:10" ht="85" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
@@ -955,7 +998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="3:10">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
@@ -967,7 +1010,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="3:10" ht="48">
+    <row r="10" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
@@ -991,7 +1034,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="48">
+    <row r="11" spans="3:10" ht="51" x14ac:dyDescent="0.2">
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1058,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="3:10">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1035,7 +1078,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="3:10" ht="32">
+    <row r="13" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1059,7 +1102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:10" ht="32">
+    <row r="14" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C14" s="5" t="s">
         <v>47</v>
       </c>
@@ -1081,7 +1124,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="3:10" ht="32">
+    <row r="15" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="7" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1160,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="3:10" ht="32">
+    <row r="17" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1141,7 +1184,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="32">
+    <row r="18" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1165,7 +1208,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="3:10">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C19" s="5" t="s">
         <v>72</v>
       </c>
@@ -1187,7 +1230,7 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="3:10">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
@@ -1199,7 +1242,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1213,7 +1256,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="3:10">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C22" s="5" t="s">
         <v>43</v>
       </c>
@@ -1227,7 +1270,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="3:10">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C23" s="5" t="s">
         <v>71</v>
       </c>
@@ -1241,7 +1284,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="3:10">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1253,7 +1296,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="3:10">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1267,7 +1310,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="3:10">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -1281,7 +1324,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="3:10" ht="32">
+    <row r="27" spans="3:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C27" s="5" t="s">
         <v>44</v>
       </c>
@@ -1303,6 +1346,50 @@
       </c>
       <c r="J27" s="5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C31" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>